<commit_message>
Need to clean data but did the count function
</commit_message>
<xml_diff>
--- a/data/Final_Dataset_ChurchLoansCapeColony.xlsx
+++ b/data/Final_Dataset_ChurchLoansCapeColony.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harriet\Documents\Economic History\ESSAY\R_History_Essay\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D186145-CB08-4BAF-8296-967D8C8269C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98436E9-4332-48BE-8015-F07AFBB479B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7C9A1DBF-A3C2-4FAF-AC33-A8302325D44B}"/>
+    <workbookView xWindow="-15" yWindow="15" windowWidth="6150" windowHeight="8460" xr2:uid="{7C9A1DBF-A3C2-4FAF-AC33-A8302325D44B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="153">
   <si>
     <t>Year</t>
   </si>
@@ -43,180 +43,30 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Surname</t>
-  </si>
-  <si>
     <t>LoanAmount</t>
   </si>
   <si>
     <t>Huguenot</t>
   </si>
   <si>
-    <t>de Lange</t>
-  </si>
-  <si>
     <t>Slave</t>
   </si>
   <si>
-    <t>van Bengalen</t>
-  </si>
-  <si>
     <t>Woman</t>
   </si>
   <si>
-    <t>Oftings</t>
-  </si>
-  <si>
-    <t>van Guinea</t>
-  </si>
-  <si>
-    <t>Brouwer</t>
-  </si>
-  <si>
     <t>du Toit</t>
   </si>
   <si>
-    <t>Viljon</t>
-  </si>
-  <si>
-    <t>Jacobs</t>
-  </si>
-  <si>
     <t>Rottinga</t>
   </si>
   <si>
     <t>Other</t>
   </si>
   <si>
-    <t>van Staaden</t>
-  </si>
-  <si>
-    <t>van Gijselen</t>
-  </si>
-  <si>
-    <t>Hendrikz</t>
-  </si>
-  <si>
-    <t>Geens</t>
-  </si>
-  <si>
-    <t>Meijijert</t>
-  </si>
-  <si>
-    <t>de Sweet</t>
-  </si>
-  <si>
-    <t>Coetzee</t>
-  </si>
-  <si>
-    <t>Vlock</t>
-  </si>
-  <si>
-    <t>van Braekel</t>
-  </si>
-  <si>
-    <t>Putter</t>
-  </si>
-  <si>
-    <t>Blank</t>
-  </si>
-  <si>
-    <t>Barentz</t>
-  </si>
-  <si>
-    <t>Cleeff</t>
-  </si>
-  <si>
-    <t>Victor</t>
-  </si>
-  <si>
-    <t>van Noorthoorn</t>
-  </si>
-  <si>
-    <t>Grimpt</t>
-  </si>
-  <si>
-    <t>Elbertz</t>
-  </si>
-  <si>
-    <t>van Oudbeijerlandt</t>
-  </si>
-  <si>
-    <t>Pretorius</t>
-  </si>
-  <si>
-    <t>van de Westhuijsen</t>
-  </si>
-  <si>
-    <t>Schalk</t>
-  </si>
-  <si>
     <t>Louwrenz</t>
   </si>
   <si>
-    <t>van Breenen</t>
-  </si>
-  <si>
-    <t>Visser</t>
-  </si>
-  <si>
-    <t>Gerbrantz</t>
-  </si>
-  <si>
-    <t>Mulder</t>
-  </si>
-  <si>
-    <t>Wuber</t>
-  </si>
-  <si>
-    <t>Mostert</t>
-  </si>
-  <si>
-    <t>Hartoog</t>
-  </si>
-  <si>
-    <t>de Groot</t>
-  </si>
-  <si>
-    <t>Rigman</t>
-  </si>
-  <si>
-    <t>Cornelisz</t>
-  </si>
-  <si>
-    <t>van Wijk</t>
-  </si>
-  <si>
-    <t>van Oldenburg</t>
-  </si>
-  <si>
-    <t>van Stralen</t>
-  </si>
-  <si>
-    <t>Wereldt</t>
-  </si>
-  <si>
-    <t>van den Brink</t>
-  </si>
-  <si>
-    <t>Steevenz</t>
-  </si>
-  <si>
-    <t>Jansz</t>
-  </si>
-  <si>
-    <t>Harts</t>
-  </si>
-  <si>
-    <t>Wirth</t>
-  </si>
-  <si>
-    <t>Meijhuijsen</t>
-  </si>
-  <si>
-    <t>Luij</t>
-  </si>
-  <si>
     <t>van Uijtregt</t>
   </si>
   <si>
@@ -226,9 +76,6 @@
     <t>Wilms</t>
   </si>
   <si>
-    <t>van Staden</t>
-  </si>
-  <si>
     <t>Gouche</t>
   </si>
   <si>
@@ -268,9 +115,6 @@
     <t>van Deventer</t>
   </si>
   <si>
-    <t>Visagie</t>
-  </si>
-  <si>
     <t>Palmars</t>
   </si>
   <si>
@@ -283,9 +127,6 @@
     <t>Siek</t>
   </si>
   <si>
-    <t>Michielse</t>
-  </si>
-  <si>
     <t>Machnie</t>
   </si>
   <si>
@@ -322,173 +163,356 @@
     <t>van Sande</t>
   </si>
   <si>
-    <t>Reijniersen</t>
-  </si>
-  <si>
-    <t>Ferdinandus</t>
-  </si>
-  <si>
-    <t>Verweij</t>
-  </si>
-  <si>
-    <t>Jans</t>
-  </si>
-  <si>
-    <t>van der Bijl</t>
-  </si>
-  <si>
-    <t>Coopman</t>
-  </si>
-  <si>
-    <t>Ras</t>
-  </si>
-  <si>
-    <t>Schrader</t>
-  </si>
-  <si>
-    <t>Rosendaal</t>
-  </si>
-  <si>
-    <t>Smient</t>
-  </si>
-  <si>
-    <t>Reijnste</t>
-  </si>
-  <si>
-    <t>Jacquerini</t>
-  </si>
-  <si>
-    <t>Adriaense</t>
-  </si>
-  <si>
-    <t>Leendertz</t>
-  </si>
-  <si>
-    <t>Broertje</t>
-  </si>
-  <si>
-    <t>Dirxe</t>
-  </si>
-  <si>
-    <t>Hendrixe</t>
-  </si>
-  <si>
-    <t>Verhagen</t>
-  </si>
-  <si>
-    <t>Steens</t>
-  </si>
-  <si>
-    <t>Janssen</t>
-  </si>
-  <si>
-    <t>Marquaart</t>
-  </si>
-  <si>
-    <t>Jacolijn</t>
-  </si>
-  <si>
-    <t>Ringel</t>
-  </si>
-  <si>
-    <t>Wolbrantz</t>
-  </si>
-  <si>
-    <t>Hanssen</t>
-  </si>
-  <si>
-    <t>Lambertz</t>
-  </si>
-  <si>
-    <t>Heere</t>
-  </si>
-  <si>
-    <t>Harmensen</t>
-  </si>
-  <si>
     <t xml:space="preserve">Slave </t>
   </si>
   <si>
-    <t>Hottentottine</t>
-  </si>
-  <si>
-    <t>van Reuven</t>
-  </si>
-  <si>
-    <t>Helmes</t>
-  </si>
-  <si>
-    <t>Willemsen</t>
-  </si>
-  <si>
-    <t>Gresnich</t>
-  </si>
-  <si>
-    <t>Claasen</t>
-  </si>
-  <si>
-    <t>Wittebol</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Jansen</t>
-  </si>
-  <si>
-    <t>Gresneg</t>
-  </si>
-  <si>
-    <t>Moijaart</t>
-  </si>
-  <si>
-    <t>Hendricx</t>
-  </si>
-  <si>
-    <t>Rijcx</t>
-  </si>
-  <si>
-    <t>Vrijsmit</t>
-  </si>
-  <si>
-    <t>Molenaar</t>
-  </si>
-  <si>
-    <t>Backer</t>
-  </si>
-  <si>
-    <t>Guchenberger</t>
-  </si>
-  <si>
-    <t>Hendrix</t>
-  </si>
-  <si>
-    <t>Greve</t>
-  </si>
-  <si>
-    <t>Sneewint</t>
-  </si>
-  <si>
-    <t>van Outbeijerlandt</t>
-  </si>
-  <si>
-    <t>Marseven</t>
-  </si>
-  <si>
-    <t>Douwes</t>
+    <t>Jan Reijniersen</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Jannetje Ferdinandus</t>
+  </si>
+  <si>
+    <t>Jan Coenrad Visser</t>
+  </si>
+  <si>
+    <t>VOC</t>
+  </si>
+  <si>
+    <t>Ghijsbert Dircks Verweij</t>
+  </si>
+  <si>
+    <t>Steven Jans</t>
+  </si>
+  <si>
+    <t>Gerrit van der Bijl</t>
+  </si>
+  <si>
+    <t>Matthijs Coopman</t>
+  </si>
+  <si>
+    <t>Hans Ras</t>
+  </si>
+  <si>
+    <t>Jan Schrader</t>
+  </si>
+  <si>
+    <t>Jacob Rosendaal</t>
+  </si>
+  <si>
+    <t>Dirck Jans Smient</t>
+  </si>
+  <si>
+    <t>Catharine Oftings</t>
+  </si>
+  <si>
+    <t>Jacques Jacquerini</t>
+  </si>
+  <si>
+    <t>Evert van Guinea</t>
+  </si>
+  <si>
+    <t>Wijnand Leendertz</t>
+  </si>
+  <si>
+    <t>Eva Hottentottine</t>
+  </si>
+  <si>
+    <t>Hans Harmensen</t>
+  </si>
+  <si>
+    <t>Willem Schalk</t>
+  </si>
+  <si>
+    <t>Jan van Reuven</t>
+  </si>
+  <si>
+    <t>Marten Leendertz</t>
+  </si>
+  <si>
+    <t>Alexander Blank</t>
+  </si>
+  <si>
+    <t>Jurriaan Heere</t>
+  </si>
+  <si>
+    <t>Pieter Visagie</t>
+  </si>
+  <si>
+    <t>Pieter Lambertz</t>
+  </si>
+  <si>
+    <t>Jan van Oldenburg</t>
+  </si>
+  <si>
+    <t>Pieter Wolbrantz</t>
+  </si>
+  <si>
+    <t>Joachim Ringel</t>
+  </si>
+  <si>
+    <t>Adriaan van Braekel</t>
+  </si>
+  <si>
+    <t>Joachim Marquaart</t>
+  </si>
+  <si>
+    <t>Pieter Janssen</t>
+  </si>
+  <si>
+    <t>Jurriaan Janssen</t>
+  </si>
+  <si>
+    <t>Jan Steens</t>
+  </si>
+  <si>
+    <t>Jan Verhagen</t>
+  </si>
+  <si>
+    <t>Thieleman Hendrixe</t>
+  </si>
+  <si>
+    <t>Cornelis Adriaense</t>
+  </si>
+  <si>
+    <t>Theunis Dirxe</t>
+  </si>
+  <si>
+    <t>Gijsbert Dirxe</t>
+  </si>
+  <si>
+    <t>Jan Broertje</t>
+  </si>
+  <si>
+    <t>Hendrick Reijnste</t>
+  </si>
+  <si>
+    <t>Hans Helmes</t>
+  </si>
+  <si>
+    <t>Arnoldus Willemsen</t>
+  </si>
+  <si>
+    <t>Gerrit Jans</t>
+  </si>
+  <si>
+    <t>Harmen Gresnich</t>
+  </si>
+  <si>
+    <t>Jacob Claasen Constapel</t>
+  </si>
+  <si>
+    <t>Jan Wittebol</t>
+  </si>
+  <si>
+    <t>Hendrick Evertsen Smith</t>
+  </si>
+  <si>
+    <t>Anthoni van Bengalen</t>
+  </si>
+  <si>
+    <t>Albert Barentz</t>
+  </si>
+  <si>
+    <t>Willem Moijaart</t>
+  </si>
+  <si>
+    <t>Hendrick Cornelis</t>
+  </si>
+  <si>
+    <t>Matjis Michielse</t>
+  </si>
+  <si>
+    <t>Barent Hendricx</t>
+  </si>
+  <si>
+    <t>Aegie Rijcx</t>
+  </si>
+  <si>
+    <t>Harmen Vrijsmit</t>
+  </si>
+  <si>
+    <t>Jan Dircxe Molenaar</t>
+  </si>
+  <si>
+    <t>Barent Backer</t>
+  </si>
+  <si>
+    <t>Herman Jansz</t>
+  </si>
+  <si>
+    <t>Francois Viljon</t>
+  </si>
+  <si>
+    <t>Louis van Bengalen</t>
+  </si>
+  <si>
+    <t>Hans Adam Guchenberger</t>
+  </si>
+  <si>
+    <t>Jan Vlock</t>
+  </si>
+  <si>
+    <t>Pieter van de Westhuijsen</t>
+  </si>
+  <si>
+    <t>Hendrick de Lange</t>
+  </si>
+  <si>
+    <t>Joannes Pretorius</t>
+  </si>
+  <si>
+    <t>Hendrick Jacobs</t>
+  </si>
+  <si>
+    <t>Jacques Jacolijn</t>
+  </si>
+  <si>
+    <t>Maarten van Staden</t>
+  </si>
+  <si>
+    <t>Leendert van Gijselen</t>
+  </si>
+  <si>
+    <t>Matthijs de Sweet</t>
+  </si>
+  <si>
+    <t>Dirk Coetzee</t>
+  </si>
+  <si>
+    <t>Gerrit van Wijnegom</t>
+  </si>
+  <si>
+    <t>Matthijs Greve</t>
+  </si>
+  <si>
+    <t>Hendrik Sneewint</t>
+  </si>
+  <si>
+    <t>Barbara Geens</t>
+  </si>
+  <si>
+    <t>Jacob Brouwer</t>
+  </si>
+  <si>
+    <t>Gerrit Victor</t>
+  </si>
+  <si>
+    <t>Hermen van Noorthoorn</t>
+  </si>
+  <si>
+    <t>Hendrik Elbertz</t>
+  </si>
+  <si>
+    <t>Jan van Outbeijerlandt</t>
+  </si>
+  <si>
+    <t>Jan van Breenen</t>
+  </si>
+  <si>
+    <t>Jan Visser</t>
+  </si>
+  <si>
+    <t>Douwes Gerbrantz</t>
+  </si>
+  <si>
+    <t>Joan Mulder</t>
+  </si>
+  <si>
+    <t>Nicholas Cleeff</t>
+  </si>
+  <si>
+    <t>Jans Wuber</t>
+  </si>
+  <si>
+    <t>Jan Mostert</t>
+  </si>
+  <si>
+    <t>Abraham Hartoog</t>
+  </si>
+  <si>
+    <t>Pieter Marseven</t>
+  </si>
+  <si>
+    <t>Simon de Groot</t>
+  </si>
+  <si>
+    <t>Jan Rigman</t>
+  </si>
+  <si>
+    <t>Willem Cornelisz</t>
+  </si>
+  <si>
+    <t>Willem van Wijk</t>
+  </si>
+  <si>
+    <t>Jeroen Douwes</t>
+  </si>
+  <si>
+    <t>Lambert Louwrenz</t>
+  </si>
+  <si>
+    <t>Hans Grimpt</t>
+  </si>
+  <si>
+    <t>Guilliam du Toit</t>
+  </si>
+  <si>
+    <t>Joris van Stralen</t>
+  </si>
+  <si>
+    <t>Willem Wereldt</t>
+  </si>
+  <si>
+    <t>Barent van den Brink</t>
+  </si>
+  <si>
+    <t>Jan Steevenz</t>
+  </si>
+  <si>
+    <t>Diderik Putter</t>
+  </si>
+  <si>
+    <t>Jan van Oudbeijerlandt</t>
+  </si>
+  <si>
+    <t>Hendrik Harts</t>
+  </si>
+  <si>
+    <t>Christoffel Wirth</t>
+  </si>
+  <si>
+    <t>Godfrid Meijhuijsen</t>
+  </si>
+  <si>
+    <t>Jan Luij</t>
+  </si>
+  <si>
+    <t>Willem Meijijert</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="3">
@@ -514,15 +538,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{88FFC59F-D641-4389-9F95-435A1F607F8D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -834,13 +860,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2258A5DD-2976-44F3-843A-EB91B8992D5C}">
-  <dimension ref="A1:D152"/>
+  <dimension ref="A1:D145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A152"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -850,10 +879,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -861,10 +890,10 @@
         <v>1670</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>43</v>
       </c>
       <c r="D2">
         <v>400</v>
@@ -875,10 +904,10 @@
         <v>1670</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="D3">
         <v>400</v>
@@ -889,10 +918,10 @@
         <v>1670</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D4">
         <v>450</v>
@@ -903,10 +932,10 @@
         <v>1670</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="D5">
         <v>600</v>
@@ -917,10 +946,10 @@
         <v>1670</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="D6">
         <v>500</v>
@@ -931,10 +960,10 @@
         <v>1670</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="D7">
         <v>600</v>
@@ -945,10 +974,10 @@
         <v>1670</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="D8">
         <v>500</v>
@@ -959,10 +988,10 @@
         <v>1670</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="D9">
         <v>580</v>
@@ -973,10 +1002,10 @@
         <v>1670</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="D10">
         <v>500</v>
@@ -987,10 +1016,10 @@
         <v>1670</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>54</v>
       </c>
       <c r="D11">
         <v>1300</v>
@@ -1001,10 +1030,10 @@
         <v>1670</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="D12">
         <v>400</v>
@@ -1015,10 +1044,10 @@
         <v>1673</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="D13">
         <v>687</v>
@@ -1029,10 +1058,10 @@
         <v>1673</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="D14">
         <v>200</v>
@@ -1043,10 +1072,10 @@
         <v>1673</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="D15">
         <v>992</v>
@@ -1057,10 +1086,10 @@
         <v>1673</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="D16">
         <v>100</v>
@@ -1071,10 +1100,10 @@
         <v>1673</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="D17">
         <v>100</v>
@@ -1085,10 +1114,10 @@
         <v>1673</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D18">
         <v>62</v>
@@ -1099,10 +1128,10 @@
         <v>1673</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D19">
         <v>300</v>
@@ -1113,13 +1142,13 @@
         <v>1673</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="D20">
-        <v>600</v>
+        <v>821</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1127,13 +1156,13 @@
         <v>1673</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="D21">
-        <v>821</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1141,13 +1170,13 @@
         <v>1673</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="D22">
-        <v>300</v>
+        <v>600</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1155,10 +1184,10 @@
         <v>1673</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="D23">
         <v>1200</v>
@@ -1169,10 +1198,10 @@
         <v>1673</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="D24">
         <v>300</v>
@@ -1183,10 +1212,10 @@
         <v>1673</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="D25">
         <v>200</v>
@@ -1197,10 +1226,10 @@
         <v>1673</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="D26">
         <v>600</v>
@@ -1211,10 +1240,10 @@
         <v>1673</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="D27">
         <v>1000</v>
@@ -1225,10 +1254,10 @@
         <v>1673</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="D28">
         <v>1000</v>
@@ -1239,10 +1268,10 @@
         <v>1673</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="D29">
         <v>300</v>
@@ -1253,10 +1282,10 @@
         <v>1673</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="D30">
         <v>400</v>
@@ -1267,10 +1296,10 @@
         <v>1673</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="D31">
         <v>200</v>
@@ -1281,10 +1310,10 @@
         <v>1673</v>
       </c>
       <c r="B32" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="D32">
         <v>500</v>
@@ -1295,10 +1324,10 @@
         <v>1673</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>117</v>
+        <v>71</v>
       </c>
       <c r="D33">
         <v>200</v>
@@ -1309,10 +1338,10 @@
         <v>1673</v>
       </c>
       <c r="B34" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="D34">
         <v>106</v>
@@ -1323,10 +1352,10 @@
         <v>1673</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="D35">
         <v>100</v>
@@ -1337,10 +1366,10 @@
         <v>1673</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="D36">
         <v>30</v>
@@ -1351,10 +1380,10 @@
         <v>1673</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="D37">
         <v>120</v>
@@ -1365,13 +1394,13 @@
         <v>1673</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="D38">
-        <v>600</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1379,13 +1408,13 @@
         <v>1673</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>122</v>
+        <v>60</v>
       </c>
       <c r="D39">
-        <v>50</v>
+        <v>785</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1393,13 +1422,13 @@
         <v>1673</v>
       </c>
       <c r="B40" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="D40">
-        <v>785</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1407,13 +1436,13 @@
         <v>1674</v>
       </c>
       <c r="B41" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41">
         <v>50</v>
-      </c>
-      <c r="D41">
-        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1421,55 +1450,55 @@
         <v>1674</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="D42">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="B43" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="D43">
-        <v>50</v>
+        <v>500</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="D44">
-        <v>200</v>
+        <v>500</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="B45" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="D45">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1477,13 +1506,13 @@
         <v>1675</v>
       </c>
       <c r="B46" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>48</v>
+        <v>88</v>
       </c>
       <c r="D46">
-        <v>300</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1491,13 +1520,13 @@
         <v>1675</v>
       </c>
       <c r="B47" t="s">
-        <v>123</v>
+        <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="D47">
-        <v>200</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1505,10 +1534,10 @@
         <v>1675</v>
       </c>
       <c r="B48" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>129</v>
+        <v>90</v>
       </c>
       <c r="D48">
         <v>100</v>
@@ -1516,30 +1545,30 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D49">
-        <v>20</v>
+        <v>300</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="B50" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="D50">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1547,13 +1576,13 @@
         <v>1676</v>
       </c>
       <c r="B51" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="D51">
-        <v>200</v>
+        <v>800</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1564,10 +1593,10 @@
         <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="D52">
-        <v>800</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1575,13 +1604,13 @@
         <v>1676</v>
       </c>
       <c r="B53" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>132</v>
+        <v>93</v>
       </c>
       <c r="D53">
-        <v>250</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1589,13 +1618,13 @@
         <v>1676</v>
       </c>
       <c r="B54" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="D54">
-        <v>500</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1603,13 +1632,13 @@
         <v>1676</v>
       </c>
       <c r="B55" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="D55">
-        <v>124</v>
+        <v>200</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1617,55 +1646,55 @@
         <v>1676</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="D56">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="B57" t="s">
         <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="D57">
-        <v>200</v>
+        <v>800</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="B58" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="D58">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="B59" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="D59">
-        <v>200</v>
+        <v>500</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1673,13 +1702,13 @@
         <v>1676</v>
       </c>
       <c r="B60" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="D60">
-        <v>800</v>
+        <v>900</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1687,13 +1716,13 @@
         <v>1677</v>
       </c>
       <c r="B61" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="D61">
-        <v>300</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1701,13 +1730,13 @@
         <v>1677</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="D62">
-        <v>500</v>
+        <v>600</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1715,13 +1744,13 @@
         <v>1677</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="D63">
-        <v>900</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1729,13 +1758,13 @@
         <v>1677</v>
       </c>
       <c r="B64" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="D64">
-        <v>1120</v>
+        <v>300</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1743,13 +1772,13 @@
         <v>1677</v>
       </c>
       <c r="B65" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="D65">
-        <v>600</v>
+        <v>450</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1757,41 +1786,41 @@
         <v>1677</v>
       </c>
       <c r="B66" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C66" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="D66">
-        <v>157</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>1677</v>
+        <v>1686</v>
       </c>
       <c r="B67" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>36</v>
+        <v>123</v>
       </c>
       <c r="D67">
-        <v>300</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>1677</v>
+        <v>1686</v>
       </c>
       <c r="B68" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D68">
-        <v>309</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1799,55 +1828,55 @@
         <v>1677</v>
       </c>
       <c r="B69" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="D69">
-        <v>450</v>
+        <v>500</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>1677</v>
+        <v>1686</v>
       </c>
       <c r="B70" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="D70">
-        <v>1142</v>
+        <v>272</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>1677</v>
+        <v>1686</v>
       </c>
       <c r="B71" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="D71">
-        <v>186</v>
+        <v>636</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>1677</v>
+        <v>1686</v>
       </c>
       <c r="B72" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="D72">
-        <v>25</v>
+        <v>672</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1855,13 +1884,13 @@
         <v>1686</v>
       </c>
       <c r="B73" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C73" t="s">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="D73">
-        <v>560</v>
+        <v>856</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1869,13 +1898,13 @@
         <v>1686</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C74" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D74">
-        <v>272</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1886,10 +1915,10 @@
         <v>8</v>
       </c>
       <c r="C75" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
       <c r="D75">
-        <v>636</v>
+        <v>236</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1897,13 +1926,13 @@
         <v>1686</v>
       </c>
       <c r="B76" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C76" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="D76">
-        <v>672</v>
+        <v>448</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1911,13 +1940,13 @@
         <v>1686</v>
       </c>
       <c r="B77" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C77" t="s">
-        <v>23</v>
+        <v>138</v>
       </c>
       <c r="D77">
-        <v>856</v>
+        <v>336</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1925,13 +1954,13 @@
         <v>1686</v>
       </c>
       <c r="B78" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C78" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="D78">
-        <v>1613</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1939,13 +1968,13 @@
         <v>1686</v>
       </c>
       <c r="B79" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C79" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="D79">
-        <v>236</v>
+        <v>254</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1953,13 +1982,13 @@
         <v>1686</v>
       </c>
       <c r="B80" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C80" t="s">
-        <v>33</v>
+        <v>126</v>
       </c>
       <c r="D80">
-        <v>448</v>
+        <v>178</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -1967,13 +1996,13 @@
         <v>1686</v>
       </c>
       <c r="B81" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C81" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D81">
-        <v>336</v>
+        <v>448</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1981,13 +2010,13 @@
         <v>1686</v>
       </c>
       <c r="B82" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C82" t="s">
-        <v>39</v>
+        <v>130</v>
       </c>
       <c r="D82">
-        <v>1062</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1995,13 +2024,13 @@
         <v>1686</v>
       </c>
       <c r="B83" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C83" t="s">
-        <v>40</v>
+        <v>131</v>
       </c>
       <c r="D83">
-        <v>254</v>
+        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2009,13 +2038,13 @@
         <v>1686</v>
       </c>
       <c r="B84" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C84" t="s">
-        <v>41</v>
+        <v>133</v>
       </c>
       <c r="D84">
-        <v>178</v>
+        <v>328</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2023,13 +2052,13 @@
         <v>1686</v>
       </c>
       <c r="B85" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C85" t="s">
-        <v>43</v>
+        <v>134</v>
       </c>
       <c r="D85">
-        <v>448</v>
+        <v>328</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2037,13 +2066,13 @@
         <v>1686</v>
       </c>
       <c r="B86" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C86" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
       <c r="D86">
-        <v>120</v>
+        <v>327</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2051,13 +2080,13 @@
         <v>1686</v>
       </c>
       <c r="B87" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C87" t="s">
-        <v>45</v>
+        <v>111</v>
       </c>
       <c r="D87">
-        <v>163</v>
+        <v>320</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2065,13 +2094,13 @@
         <v>1686</v>
       </c>
       <c r="B88" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C88" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="D88">
-        <v>328</v>
+        <v>539</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2079,13 +2108,13 @@
         <v>1686</v>
       </c>
       <c r="B89" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C89" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="D89">
-        <v>328</v>
+        <v>3285</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2093,55 +2122,55 @@
         <v>1686</v>
       </c>
       <c r="B90" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C90" t="s">
-        <v>49</v>
+        <v>137</v>
       </c>
       <c r="D90">
-        <v>327</v>
+        <v>50</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="B91" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C91" t="s">
-        <v>63</v>
+        <v>140</v>
       </c>
       <c r="D91">
-        <v>320</v>
+        <v>212</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="B92" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C92" t="s">
-        <v>18</v>
+        <v>141</v>
       </c>
       <c r="D92">
-        <v>3285</v>
+        <v>313</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="B93" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C93" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D93">
-        <v>50</v>
+        <v>208</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2149,13 +2178,13 @@
         <v>1687</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C94" t="s">
-        <v>12</v>
+        <v>143</v>
       </c>
       <c r="D94">
-        <v>212</v>
+        <v>354</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2163,83 +2192,83 @@
         <v>1687</v>
       </c>
       <c r="B95" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C95" t="s">
-        <v>51</v>
+        <v>144</v>
       </c>
       <c r="D95">
-        <v>313</v>
+        <v>601</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="B96" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C96" t="s">
-        <v>52</v>
+        <v>145</v>
       </c>
       <c r="D96">
-        <v>208</v>
+        <v>652</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>1687</v>
+        <v>1676</v>
       </c>
       <c r="B97" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C97" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="D97">
-        <v>354</v>
+        <v>400</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="B98" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C98" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="D98">
-        <v>601</v>
+        <v>224</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>1688</v>
+        <v>1686</v>
       </c>
       <c r="B99" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C99" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="D99">
-        <v>652</v>
+        <v>444</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>1688</v>
+        <v>1686</v>
       </c>
       <c r="B100" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C100" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
       <c r="D100">
-        <v>672</v>
+        <v>928</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2247,13 +2276,13 @@
         <v>1688</v>
       </c>
       <c r="B101" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C101" t="s">
-        <v>29</v>
+        <v>147</v>
       </c>
       <c r="D101">
-        <v>224</v>
+        <v>318</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2261,13 +2290,13 @@
         <v>1688</v>
       </c>
       <c r="B102" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C102" t="s">
-        <v>31</v>
+        <v>148</v>
       </c>
       <c r="D102">
-        <v>730</v>
+        <v>212</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2275,13 +2304,13 @@
         <v>1688</v>
       </c>
       <c r="B103" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C103" t="s">
-        <v>42</v>
+        <v>149</v>
       </c>
       <c r="D103">
-        <v>636</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2289,41 +2318,41 @@
         <v>1688</v>
       </c>
       <c r="B104" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C104" t="s">
-        <v>56</v>
+        <v>150</v>
       </c>
       <c r="D104">
-        <v>318</v>
+        <v>70</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="B105" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C105" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="D105">
-        <v>212</v>
+        <v>672</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="B106" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C106" t="s">
-        <v>58</v>
+        <v>151</v>
       </c>
       <c r="D106">
-        <v>1045</v>
+        <v>848</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -2331,181 +2360,181 @@
         <v>1688</v>
       </c>
       <c r="B107" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C107" t="s">
-        <v>59</v>
+        <v>146</v>
       </c>
       <c r="D107">
-        <v>70</v>
+        <v>168</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>1689</v>
+        <v>1677</v>
       </c>
       <c r="B108" t="s">
         <v>8</v>
       </c>
       <c r="C108" t="s">
-        <v>15</v>
+        <v>101</v>
       </c>
       <c r="D108">
-        <v>672</v>
+        <v>317</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109">
-        <v>1689</v>
+      <c r="A109" t="s">
+        <v>152</v>
       </c>
       <c r="B109" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C109" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D109">
-        <v>354</v>
+        <v>408</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110">
-        <v>1689</v>
+      <c r="A110" t="s">
+        <v>152</v>
       </c>
       <c r="B110" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C110" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D110">
-        <v>3441</v>
+        <v>477</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111">
-        <v>1689</v>
+      <c r="A111" t="s">
+        <v>152</v>
       </c>
       <c r="B111" t="s">
-        <v>16</v>
-      </c>
-      <c r="C111" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D111">
-        <v>202</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>1689</v>
+        <v>1706</v>
       </c>
       <c r="B112" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C112" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D112">
-        <v>848</v>
+        <v>725</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>1689</v>
+        <v>1706</v>
       </c>
       <c r="B113" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C113" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D113">
-        <v>177</v>
+        <v>613</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>1689</v>
+        <v>1706</v>
       </c>
       <c r="B114" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C114" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D114">
-        <v>390</v>
+        <v>607</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>1689</v>
+        <v>1706</v>
       </c>
       <c r="B115" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C115" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="D115">
-        <v>708</v>
+        <v>224</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>1689</v>
+        <v>1706</v>
       </c>
       <c r="B116" t="s">
+        <v>3</v>
+      </c>
+      <c r="C116" t="s">
         <v>16</v>
       </c>
-      <c r="C116" t="s">
-        <v>55</v>
-      </c>
       <c r="D116">
-        <v>226</v>
+        <v>336</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>1690</v>
+        <v>1706</v>
       </c>
       <c r="B117" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C117" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="D117">
-        <v>408</v>
+        <v>472</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>1690</v>
+        <v>1706</v>
       </c>
       <c r="B118" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C118" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="D118">
-        <v>477</v>
+        <v>708</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>1690</v>
+        <v>1706</v>
       </c>
       <c r="B119" t="s">
         <v>8</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>62</v>
+      <c r="C119" t="s">
+        <v>19</v>
       </c>
       <c r="D119">
-        <v>1000</v>
+        <v>763</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2513,13 +2542,13 @@
         <v>1706</v>
       </c>
       <c r="B120" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C120" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="D120">
-        <v>725</v>
+        <v>780</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2527,13 +2556,13 @@
         <v>1706</v>
       </c>
       <c r="B121" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C121" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="D121">
-        <v>613</v>
+        <v>372</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2541,13 +2570,13 @@
         <v>1706</v>
       </c>
       <c r="B122" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C122" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="D122">
-        <v>607</v>
+        <v>590</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2555,13 +2584,13 @@
         <v>1706</v>
       </c>
       <c r="B123" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C123" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D123">
-        <v>224</v>
+        <v>254</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2569,13 +2598,13 @@
         <v>1706</v>
       </c>
       <c r="B124" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C124" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="D124">
-        <v>336</v>
+        <v>496</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2583,13 +2612,13 @@
         <v>1706</v>
       </c>
       <c r="B125" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C125" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="D125">
-        <v>472</v>
+        <v>496</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -2597,13 +2626,13 @@
         <v>1706</v>
       </c>
       <c r="B126" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C126" t="s">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="D126">
-        <v>708</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -2611,13 +2640,13 @@
         <v>1706</v>
       </c>
       <c r="B127" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C127" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="D127">
-        <v>763</v>
+        <v>533</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -2625,13 +2654,13 @@
         <v>1706</v>
       </c>
       <c r="B128" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C128" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="D128">
-        <v>780</v>
+        <v>879</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -2639,13 +2668,13 @@
         <v>1706</v>
       </c>
       <c r="B129" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C129" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="D129">
-        <v>372</v>
+        <v>708</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -2653,13 +2682,13 @@
         <v>1706</v>
       </c>
       <c r="B130" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C130" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="D130">
-        <v>590</v>
+        <v>224</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -2667,13 +2696,13 @@
         <v>1706</v>
       </c>
       <c r="B131" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C131" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="D131">
-        <v>254</v>
+        <v>372</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -2681,13 +2710,13 @@
         <v>1706</v>
       </c>
       <c r="B132" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C132" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D132">
-        <v>496</v>
+        <v>248</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -2695,13 +2724,13 @@
         <v>1706</v>
       </c>
       <c r="B133" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C133" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="D133">
-        <v>496</v>
+        <v>708</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -2709,13 +2738,13 @@
         <v>1706</v>
       </c>
       <c r="B134" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C134" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="D134">
-        <v>1028</v>
+        <v>496</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -2723,13 +2752,13 @@
         <v>1706</v>
       </c>
       <c r="B135" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C135" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="D135">
-        <v>533</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -2737,242 +2766,144 @@
         <v>1706</v>
       </c>
       <c r="B136" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C136" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="D136">
-        <v>879</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>1706</v>
+        <v>1708</v>
       </c>
       <c r="B137" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C137" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="D137">
-        <v>708</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>1706</v>
+        <v>1709</v>
       </c>
       <c r="B138" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C138" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="D138">
-        <v>224</v>
+        <v>316</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>1706</v>
+        <v>1709</v>
       </c>
       <c r="B139" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C139" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="D139">
-        <v>372</v>
+        <v>611</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>1706</v>
+        <v>1709</v>
       </c>
       <c r="B140" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C140" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="D140">
-        <v>248</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>1706</v>
+        <v>1709</v>
       </c>
       <c r="B141" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C141" t="s">
-        <v>85</v>
+        <v>39</v>
       </c>
       <c r="D141">
-        <v>708</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>1706</v>
+        <v>1710</v>
       </c>
       <c r="B142" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C142" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="D142">
-        <v>496</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>1706</v>
+        <v>1710</v>
       </c>
       <c r="B143" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C143" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="D143">
-        <v>2138</v>
+        <v>832</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>1706</v>
+        <v>1710</v>
       </c>
       <c r="B144" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C144" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="D144">
-        <v>1240</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>1708</v>
+        <v>1686</v>
       </c>
       <c r="B145" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C145" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="D145">
-        <v>1507</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146">
-        <v>1709</v>
-      </c>
-      <c r="B146" t="s">
-        <v>16</v>
-      </c>
-      <c r="C146" t="s">
-        <v>90</v>
-      </c>
-      <c r="D146">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147">
-        <v>1709</v>
-      </c>
-      <c r="B147" t="s">
-        <v>16</v>
-      </c>
-      <c r="C147" t="s">
-        <v>91</v>
-      </c>
-      <c r="D147">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148">
-        <v>1709</v>
-      </c>
-      <c r="B148" t="s">
-        <v>16</v>
-      </c>
-      <c r="C148" t="s">
-        <v>88</v>
-      </c>
-      <c r="D148">
-        <v>1573</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149">
-        <v>1709</v>
-      </c>
-      <c r="B149" t="s">
-        <v>16</v>
-      </c>
-      <c r="C149" t="s">
-        <v>92</v>
-      </c>
-      <c r="D149">
-        <v>2039</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150">
-        <v>1710</v>
-      </c>
-      <c r="B150" t="s">
-        <v>16</v>
-      </c>
-      <c r="C150" t="s">
-        <v>93</v>
-      </c>
-      <c r="D150">
-        <v>2103</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151">
-        <v>1710</v>
-      </c>
-      <c r="B151" t="s">
-        <v>16</v>
-      </c>
-      <c r="C151" t="s">
-        <v>89</v>
-      </c>
-      <c r="D151">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152">
-        <v>1710</v>
-      </c>
-      <c r="B152" t="s">
-        <v>16</v>
-      </c>
-      <c r="C152" t="s">
-        <v>94</v>
-      </c>
-      <c r="D152">
-        <v>1033</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D152">
-    <sortCondition ref="A2:A152"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D144">
+    <sortCondition ref="A2:A144"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>